<commit_message>
Adding balance and debt classes
</commit_message>
<xml_diff>
--- a/simfin/debt/historical_accounts.xlsx
+++ b/simfin/debt/historical_accounts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\80002036\Documents\GitHub\simfin\simfin\debt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6515190C-9489-4D2E-BE8F-E256D2001B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2100409-750A-4BBE-9824-A964F7DEAC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3390" yWindow="14290" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="2" r:id="rId1"/>
@@ -36,21 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>account</t>
   </si>
   <si>
-    <t>debt_balance_start</t>
-  </si>
-  <si>
     <t>debt_repay</t>
-  </si>
-  <si>
-    <t>debt_balance_end</t>
-  </si>
-  <si>
-    <t>gross_debt_reduct</t>
   </si>
   <si>
     <t>gross_debt</t>
@@ -60,6 +51,9 @@
   </si>
   <si>
     <t>e_cycle</t>
+  </si>
+  <si>
+    <t>direct_debt</t>
   </si>
 </sst>
 </file>
@@ -433,10 +427,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Feuil2"/>
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A8" sqref="A8:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -452,10 +446,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D1">
         <v>2006</v>
@@ -516,56 +510,58 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2"/>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2">
-        <v>88582</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>110437</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>118089</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>133224</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>136074</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>147748</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>158887</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>168612</v>
+        <v>1000</v>
       </c>
       <c r="M2">
-        <v>174085</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>182723</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>185124</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>189366</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>191984</v>
+        <v>8000</v>
       </c>
       <c r="R2">
-        <v>189029</v>
+        <v>2000</v>
       </c>
       <c r="S2">
-        <v>192975</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -574,57 +570,57 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>88582</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>108585</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>118089</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>133224</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>136074</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>147748</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>158887</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>168616</v>
       </c>
       <c r="L3">
-        <v>1000</v>
+        <v>174085</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>182723</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>185124</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>189366</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>191984</v>
       </c>
       <c r="Q3">
-        <v>8000</v>
-      </c>
-      <c r="R3">
-        <v>2000</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
+        <v>189029</v>
+      </c>
+      <c r="R3" s="3">
+        <v>192975</v>
+      </c>
+      <c r="S3" s="3">
+        <v>218583</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -633,179 +629,73 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>88582</v>
+        <v>125764</v>
       </c>
       <c r="E4">
-        <v>108585</v>
+        <v>141597</v>
       </c>
       <c r="F4">
-        <v>118089</v>
+        <v>148015</v>
       </c>
       <c r="G4">
-        <v>133224</v>
+        <v>159980</v>
       </c>
       <c r="H4">
-        <v>136074</v>
+        <v>163318</v>
       </c>
       <c r="I4">
-        <v>147748</v>
+        <v>173436</v>
       </c>
       <c r="J4">
-        <v>158887</v>
+        <v>183384</v>
       </c>
       <c r="K4">
-        <v>168616</v>
+        <v>191756</v>
       </c>
       <c r="L4">
-        <v>174085</v>
+        <v>197098</v>
       </c>
       <c r="M4">
-        <v>182723</v>
+        <v>203957</v>
       </c>
       <c r="N4">
-        <v>185124</v>
+        <v>203347</v>
       </c>
       <c r="O4">
-        <v>189366</v>
+        <v>203490</v>
       </c>
       <c r="P4">
-        <v>191984</v>
+        <v>201071</v>
       </c>
       <c r="Q4">
-        <v>189029</v>
+        <v>199098</v>
       </c>
       <c r="R4" s="3">
-        <v>192975</v>
+        <v>198792</v>
       </c>
       <c r="S4" s="3">
-        <v>218583</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>3429</v>
-      </c>
-      <c r="E5">
-        <v>6100</v>
-      </c>
-      <c r="F5">
-        <v>2438</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>4980</v>
-      </c>
-      <c r="I5">
-        <v>5881</v>
-      </c>
-      <c r="J5">
-        <v>5799</v>
-      </c>
-      <c r="K5">
-        <v>4964</v>
-      </c>
-      <c r="L5">
-        <v>6947</v>
-      </c>
-      <c r="M5">
-        <v>10027</v>
-      </c>
-      <c r="N5">
-        <v>8821</v>
-      </c>
-      <c r="O5">
-        <v>8190</v>
-      </c>
-      <c r="P5">
-        <v>9965</v>
-      </c>
-      <c r="Q5">
-        <v>6159</v>
-      </c>
-      <c r="R5" s="3">
-        <v>7988</v>
-      </c>
-      <c r="S5" s="3">
-        <v>4292</v>
-      </c>
-    </row>
+        <v>218957</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>125764</v>
-      </c>
-      <c r="E6">
-        <v>141597</v>
-      </c>
-      <c r="F6">
-        <v>148015</v>
-      </c>
-      <c r="G6">
-        <v>159980</v>
-      </c>
-      <c r="H6">
-        <v>163318</v>
-      </c>
-      <c r="I6">
-        <v>173436</v>
-      </c>
-      <c r="J6">
-        <v>183384</v>
-      </c>
-      <c r="K6">
-        <v>191756</v>
-      </c>
-      <c r="L6">
-        <v>197098</v>
-      </c>
-      <c r="M6">
-        <v>203957</v>
-      </c>
-      <c r="N6">
-        <v>203347</v>
-      </c>
-      <c r="O6">
-        <v>203490</v>
-      </c>
-      <c r="P6">
-        <v>201071</v>
-      </c>
-      <c r="Q6">
-        <v>199098</v>
-      </c>
-      <c r="R6" s="3">
-        <v>198792</v>
-      </c>
-      <c r="S6" s="3">
-        <v>218957</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -1022,18 +912,6 @@
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>